<commit_message>
Changes to experiment with new learning rate
</commit_message>
<xml_diff>
--- a/LJ Experiments.xlsx
+++ b/LJ Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhvan\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Speech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FA87DC-9F38-4D23-906B-2CCBDC79D806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E09EA44-484F-4DA8-A684-A82AB6658B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="12">
   <si>
     <t>&lt;__main__.DisplayOutputs object at 0x7fe956d0d0a0&gt;</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>WER-97%</t>
+  </si>
+  <si>
+    <t>&lt;__main__.DisplayOutputs object at 0x7ff55e4a7640&gt;</t>
+  </si>
+  <si>
+    <t>WER - 92%</t>
   </si>
 </sst>
 </file>
@@ -2500,6 +2506,1021 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-NZ"/>
+              <a:t>WER</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40 + 200 epoches'!$B$2:$B$242</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="241"/>
+                <c:pt idx="0">
+                  <c:v>0.92883053883736211</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95301067749456425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.94798907163705559</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98273889977782758</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94776322957973513</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.97286088162113959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94645358473562524</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99430953302103875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98999608887057644</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.94278365608891879</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99451893425169813</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97928995703878374</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.91581302380224172</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.95273135975258616</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0762325100925521</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.060029452254281</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.047360008662241</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.040048643380717</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.005064679365786</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99741920698508668</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0325167929348611</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.000493055546547</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.9913340475532203</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.93569590437049688</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94884032840023147</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.95151073910765382</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.94032286613302474</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.93357215502868607</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.91344161007418656</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.92787622960542127</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.015057670217665</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.024682740537612</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98834297732050913</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.97045652609339894</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0106727175288031</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.96392782231215857</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.90791667219907279</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.93819699819198166</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.93392749865246849</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.93680632885453319</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.93216140988423846</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.90959096335922007</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.90034417086447405</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.88861969173451916</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.93221850735759881</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.90549879553731749</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.94416787191600593</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.95008178309971203</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.90083154530544451</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.96957797911441224</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.98532774337596385</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.93844330138099352</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.94679771297738879</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.91919947947761249</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.93912437357466649</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.91555487786576484</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.92070220776261036</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.89739615264593209</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.90324210728335519</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.91035721193414787</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.91034633720487279</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.88596064172957256</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.93523076663548754</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.91684680352736359</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.95167691565980717</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.92433510938745678</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.94103879603170115</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.90529483172226466</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.92064053230629783</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89377064273206352</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.87292158776997753</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.8400085323856753</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.88935710828608472</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.88008069076003648</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.97029404926401464</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.92027103577067493</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.88625455231886041</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.86516961210364018</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.85749087145660663</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.90930955201221098</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.89528076793947808</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.89856979536178638</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.90321868723198662</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.94368585524746396</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.92812337175933945</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.93443966655267874</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.96415133116339558</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.92089798303989756</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.91930360822056179</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.9080257489413911</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.90577019462786235</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.87605462531295264</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.87514097265511626</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.88259059382610183</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.87378051845664462</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.89205337976966226</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.89671860942261161</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.88854373879703052</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.88609954316476014</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.88168717666760099</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.91330513107945477</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.8998291819876969</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.89523095528950103</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.88398302590649858</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.88814154326063843</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.89043312440459021</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.89208691060672729</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>0.89666280082536609</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>0.89071046117211605</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>0.90559366048026746</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.89898180467613631</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.91042678330861504</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0.90823827510787847</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.91449633995969337</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.9322179370167285</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0.9125984822803489</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.92391087479935463</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0.92207808025912474</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.94297402765323401</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.92756596452939888</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.92688251644900987</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.92904746130451743</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0.92971498702592248</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.94208982733062552</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0.93284745900001631</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.93930649343667494</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0.92195576630218223</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0.91965207036361785</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.91696234018806622</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.91894625825418619</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0.9168913031669842</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.90863191218633044</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0.91051951400799558</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.90094851760427586</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0.91304264284741843</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0.90232601502065846</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0.91889878525890989</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0.91888270622784318</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0.91320100043148955</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0.90962483355169421</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.91222829143282236</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.92334274121914717</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0.91741621523287853</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0.91434341476058156</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0.92305575798179629</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.90720550054472526</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0.92298542146444884</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.93006411563904823</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>0.93126600372940604</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.92311138087381339</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>0.91189751315319212</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.92805690907856453</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.93625764665981392</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.92190324352688657</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.92103955203579724</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.91884149074606392</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.92221486692403043</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.92700445949087418</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>0.91688371105151123</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>0.91587520974889247</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>0.91679195668963909</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.92127425051296563</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.90823845112707946</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>0.9177578657805483</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>0.93002559691716535</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>0.91236855777575121</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.91085340626059974</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>0.91006942461724305</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.91364485822968333</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.91503443332849765</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>0.92102883457783302</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.91902576819976667</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.91416160229010435</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.91284593561538241</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.91145588262037025</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.91728601610587179</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.93215291981057025</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.91642168191952678</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.92590616689034344</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>0.9173827453126554</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>0.92327914332254002</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.93081679362513614</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.93128191870071941</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.93445276269079269</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>0.94067686042853738</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>0.94164029916371528</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>0.93626591456138941</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.93564887173605071</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.9525288892933127</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.94151870870592635</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.92248611301214634</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.93409942659914424</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>0.93272484631831376</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>0.92506859631831373</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>0.91985784747978594</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.93303486615958386</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>0.92576794362875281</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.93011302199277301</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.92902085027560144</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0.92807590979941079</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.92807590979941079</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.93449306785864206</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.90360820073454196</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.89409825585242297</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.92046585473033449</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.86389243860717535</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>0.8686002481487024</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.960981520972084</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>0.88236883671915545</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>0.94037753533400348</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.93480862179883772</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>0.90041068067746644</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.90339134058022597</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.92156489823471899</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.89096992301644784</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>0.91458785845994972</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>0.96733739706362676</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.93642956015465162</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>0.91399646374299659</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.99418237061668335</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>0.9697711650140316</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0.921411876361515</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.9058232889643244</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.952449841400138</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.92064278092431384</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>0.89939522729142551</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.91687705786506268</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>0.92593348635421113</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>0.94284649725435432</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.96499812105585892</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>0.8818035270297736</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.9271677149820341</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>0.95786011815329675</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.94032607334928631</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>0.91728714202352135</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>0.93412014207143967</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.93727835304354479</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>0.95573170953324882</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>0.91509921544190231</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>0.88184730225393815</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.98345618415923985</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7D63-4768-A34C-A9F805E19BCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="809612991"/>
+        <c:axId val="809611743"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="809612991"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="809611743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="809611743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="809612991"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2660,6 +3681,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4209,6 +5270,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5184,6 +6761,97 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>307181</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>135731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>345281</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>164306</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1978D0BB-9ED2-FF77-EC03-71458F8F0D68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>71438</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B995201-0252-5259-60D5-F69FDA511A09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7410450" y="228600"/>
+          <a:ext cx="4319588" cy="3239691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6995,7 +8663,7 @@
   <dimension ref="A1:D202"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8966,14 +10634,1947 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261AB831-E7E2-489B-93E7-0AC004FB33D1}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E242"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.92883053883736211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.95301067749456425</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.94798907163705559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.98273889977782758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.94776322957973513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.97286088162113959</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.94645358473562524</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.99430953302103875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.98999608887057644</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.94278365608891879</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.99451893425169813</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.97928995703878374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.91581302380224172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.95273135975258616</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1.0762325100925521</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1.060029452254281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1.047360008662241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1.040048643380717</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1.005064679365786</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.99741920698508668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1.0325167929348611</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1.000493055546547</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.9913340475532203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0.93569590437049688</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>0.94884032840023147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>0.95151073910765382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>0.94032286613302474</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>0.93357215502868607</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.91344161007418656</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>0.92787622960542127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>1.015057670217665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>1.024682740537612</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>0.98834297732050913</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>0.97045652609339894</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>1.0106727175288031</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>0.96392782231215857</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>0.90791667219907279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>0.93819699819198166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>0.93392749865246849</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>0.93680632885453319</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>0.93216140988423846</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>0.90959096335922007</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>0.90034417086447405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>0.88861969173451916</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>0.93221850735759881</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>0.90549879553731749</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>0.94416787191600593</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>0.95008178309971203</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>0.90083154530544451</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A51">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>0.96957797911441224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A52">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>0.98532774337596385</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>0.93844330138099352</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>0.94679771297738879</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>0.91919947947761249</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>0.93912437357466649</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>0.91555487786576484</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>0.92070220776261036</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>0.89739615264593209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>0.90324210728335519</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>0.91035721193414787</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>0.91034633720487279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>0.88596064172957256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>0.93523076663548754</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>0.91684680352736359</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>0.95167691565980717</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>0.92433510938745678</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>0.94103879603170115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>0.90529483172226466</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>0.92064053230629783</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0.89377064273206352</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>0.87292158776997753</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>0.8400085323856753</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>0.88935710828608472</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>0.88008069076003648</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>0.97029404926401464</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>0.92027103577067493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>0.88625455231886041</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>0.86516961210364018</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>0.85749087145660663</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>0.90930955201221098</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>0.89528076793947808</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>0.89856979536178638</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>0.90321868723198662</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>0.94368585524746396</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>0.92812337175933945</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>0.93443966655267874</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>0.96415133116339558</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>0.92089798303989756</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>0.91930360822056179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>0.9080257489413911</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>0.90577019462786235</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>0.87605462531295264</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>0.87514097265511626</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>0.88259059382610183</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>0.87378051845664462</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>0.89205337976966226</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>0.89671860942261161</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>0.88854373879703052</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>0.88609954316476014</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>0.88168717666760099</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>0.91330513107945477</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>0.8998291819876969</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>0.89523095528950103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>0.88398302590649858</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>0.88814154326063843</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>0.89043312440459021</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>0.89208691060672729</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>0.89666280082536609</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>0.89071046117211605</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A111">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>0.90559366048026746</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A112">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>0.89898180467613631</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A113">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>0.91042678330861504</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A114">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>0.90823827510787847</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A115">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>0.91449633995969337</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A116">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>0.9322179370167285</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A117">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>0.9125984822803489</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A118">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>0.92391087479935463</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A119">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>0.92207808025912474</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A120">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>0.94297402765323401</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A121">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>0.92756596452939888</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A122">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>0.92688251644900987</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A123">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>0.92904746130451743</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A124">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>0.92971498702592248</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A125">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>0.94208982733062552</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A126">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>0.93284745900001631</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A127">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>0.93930649343667494</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A128">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>0.92195576630218223</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A129">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>0.91965207036361785</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A130">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>0.91696234018806622</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A131">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>0.91894625825418619</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A132">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>0.9168913031669842</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A133">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>0.90863191218633044</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A134">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>0.91051951400799558</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A135">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>0.90094851760427586</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A136">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>0.91304264284741843</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A137">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>0.90232601502065846</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A138">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>0.91889878525890989</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A139">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>0.91888270622784318</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A140">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>0.91320100043148955</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A141">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>0.90962483355169421</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A142">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>0.91222829143282236</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A143">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>0.92334274121914717</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A144">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>0.91741621523287853</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A145">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>0.91434341476058156</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A146">
+        <v>144</v>
+      </c>
+      <c r="B146">
+        <v>0.92305575798179629</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A147">
+        <v>145</v>
+      </c>
+      <c r="B147">
+        <v>0.90720550054472526</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A148">
+        <v>146</v>
+      </c>
+      <c r="B148">
+        <v>0.92298542146444884</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A149">
+        <v>147</v>
+      </c>
+      <c r="B149">
+        <v>0.93006411563904823</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A150">
+        <v>148</v>
+      </c>
+      <c r="B150">
+        <v>0.93126600372940604</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A151">
+        <v>149</v>
+      </c>
+      <c r="B151">
+        <v>0.92311138087381339</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A152">
+        <v>150</v>
+      </c>
+      <c r="B152">
+        <v>0.91189751315319212</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A153">
+        <v>151</v>
+      </c>
+      <c r="B153">
+        <v>0.92805690907856453</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154">
+        <v>0.93625764665981392</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155">
+        <v>0.92190324352688657</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156">
+        <v>0.92103955203579724</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A157">
+        <v>155</v>
+      </c>
+      <c r="B157">
+        <v>0.91884149074606392</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A158">
+        <v>156</v>
+      </c>
+      <c r="B158">
+        <v>0.92221486692403043</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A159">
+        <v>157</v>
+      </c>
+      <c r="B159">
+        <v>0.92700445949087418</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A160">
+        <v>158</v>
+      </c>
+      <c r="B160">
+        <v>0.91688371105151123</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A161">
+        <v>159</v>
+      </c>
+      <c r="B161">
+        <v>0.91587520974889247</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A162">
+        <v>160</v>
+      </c>
+      <c r="B162">
+        <v>0.91679195668963909</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A163">
+        <v>161</v>
+      </c>
+      <c r="B163">
+        <v>0.92127425051296563</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A164">
+        <v>162</v>
+      </c>
+      <c r="B164">
+        <v>0.90823845112707946</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A165">
+        <v>163</v>
+      </c>
+      <c r="B165">
+        <v>0.9177578657805483</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A166">
+        <v>164</v>
+      </c>
+      <c r="B166">
+        <v>0.93002559691716535</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A167">
+        <v>165</v>
+      </c>
+      <c r="B167">
+        <v>0.91236855777575121</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A168">
+        <v>166</v>
+      </c>
+      <c r="B168">
+        <v>0.91085340626059974</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A169">
+        <v>167</v>
+      </c>
+      <c r="B169">
+        <v>0.91006942461724305</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A170">
+        <v>168</v>
+      </c>
+      <c r="B170">
+        <v>0.91364485822968333</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A171">
+        <v>169</v>
+      </c>
+      <c r="B171">
+        <v>0.91503443332849765</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A172">
+        <v>170</v>
+      </c>
+      <c r="B172">
+        <v>0.92102883457783302</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A173">
+        <v>171</v>
+      </c>
+      <c r="B173">
+        <v>0.91902576819976667</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A174">
+        <v>172</v>
+      </c>
+      <c r="B174">
+        <v>0.91416160229010435</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A175">
+        <v>173</v>
+      </c>
+      <c r="B175">
+        <v>0.91284593561538241</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A176">
+        <v>174</v>
+      </c>
+      <c r="B176">
+        <v>0.91145588262037025</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A177">
+        <v>175</v>
+      </c>
+      <c r="B177">
+        <v>0.91728601610587179</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A178">
+        <v>176</v>
+      </c>
+      <c r="B178">
+        <v>0.93215291981057025</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A179">
+        <v>177</v>
+      </c>
+      <c r="B179">
+        <v>0.91642168191952678</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A180">
+        <v>178</v>
+      </c>
+      <c r="B180">
+        <v>0.92590616689034344</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A181">
+        <v>179</v>
+      </c>
+      <c r="B181">
+        <v>0.9173827453126554</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A182">
+        <v>180</v>
+      </c>
+      <c r="B182">
+        <v>0.92327914332254002</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A183">
+        <v>181</v>
+      </c>
+      <c r="B183">
+        <v>0.93081679362513614</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A184">
+        <v>182</v>
+      </c>
+      <c r="B184">
+        <v>0.93128191870071941</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A185">
+        <v>183</v>
+      </c>
+      <c r="B185">
+        <v>0.93445276269079269</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A186">
+        <v>184</v>
+      </c>
+      <c r="B186">
+        <v>0.94067686042853738</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A187">
+        <v>185</v>
+      </c>
+      <c r="B187">
+        <v>0.94164029916371528</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A188">
+        <v>186</v>
+      </c>
+      <c r="B188">
+        <v>0.93626591456138941</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A189">
+        <v>187</v>
+      </c>
+      <c r="B189">
+        <v>0.93564887173605071</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A190">
+        <v>188</v>
+      </c>
+      <c r="B190">
+        <v>0.9525288892933127</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A191">
+        <v>189</v>
+      </c>
+      <c r="B191">
+        <v>0.94151870870592635</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A192">
+        <v>190</v>
+      </c>
+      <c r="B192">
+        <v>0.92248611301214634</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A193">
+        <v>191</v>
+      </c>
+      <c r="B193">
+        <v>0.93409942659914424</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A194">
+        <v>192</v>
+      </c>
+      <c r="B194">
+        <v>0.93272484631831376</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A195">
+        <v>193</v>
+      </c>
+      <c r="B195">
+        <v>0.92506859631831373</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A196">
+        <v>194</v>
+      </c>
+      <c r="B196">
+        <v>0.91985784747978594</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A197">
+        <v>195</v>
+      </c>
+      <c r="B197">
+        <v>0.93303486615958386</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A198">
+        <v>196</v>
+      </c>
+      <c r="B198">
+        <v>0.92576794362875281</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A199">
+        <v>197</v>
+      </c>
+      <c r="B199">
+        <v>0.93011302199277301</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A200">
+        <v>198</v>
+      </c>
+      <c r="B200">
+        <v>0.92902085027560144</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A201">
+        <v>199</v>
+      </c>
+      <c r="B201">
+        <v>0.92807590979941079</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A202" t="s">
+        <v>10</v>
+      </c>
+      <c r="B202">
+        <v>0.92807590979941079</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+      <c r="B203">
+        <v>0.93449306785864206</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A204" t="s">
+        <v>10</v>
+      </c>
+      <c r="B204">
+        <v>0.90360820073454196</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A205" t="s">
+        <v>10</v>
+      </c>
+      <c r="B205">
+        <v>0.89409825585242297</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A206" t="s">
+        <v>10</v>
+      </c>
+      <c r="B206">
+        <v>0.92046585473033449</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A207" t="s">
+        <v>10</v>
+      </c>
+      <c r="B207">
+        <v>0.86389243860717535</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A208" t="s">
+        <v>10</v>
+      </c>
+      <c r="B208">
+        <v>0.8686002481487024</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A209" t="s">
+        <v>10</v>
+      </c>
+      <c r="B209">
+        <v>0.960981520972084</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A210" t="s">
+        <v>10</v>
+      </c>
+      <c r="B210">
+        <v>0.88236883671915545</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A211" t="s">
+        <v>10</v>
+      </c>
+      <c r="B211">
+        <v>0.94037753533400348</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A212" t="s">
+        <v>10</v>
+      </c>
+      <c r="B212">
+        <v>0.93480862179883772</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A213" t="s">
+        <v>10</v>
+      </c>
+      <c r="B213">
+        <v>0.90041068067746644</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A214" t="s">
+        <v>10</v>
+      </c>
+      <c r="B214">
+        <v>0.90339134058022597</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A215" t="s">
+        <v>10</v>
+      </c>
+      <c r="B215">
+        <v>0.92156489823471899</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A216" t="s">
+        <v>10</v>
+      </c>
+      <c r="B216">
+        <v>0.89096992301644784</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A217" t="s">
+        <v>10</v>
+      </c>
+      <c r="B217">
+        <v>0.91458785845994972</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A218" t="s">
+        <v>10</v>
+      </c>
+      <c r="B218">
+        <v>0.96733739706362676</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A219" t="s">
+        <v>10</v>
+      </c>
+      <c r="B219">
+        <v>0.93642956015465162</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A220" t="s">
+        <v>10</v>
+      </c>
+      <c r="B220">
+        <v>0.91399646374299659</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A221" t="s">
+        <v>10</v>
+      </c>
+      <c r="B221">
+        <v>0.99418237061668335</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A222" t="s">
+        <v>10</v>
+      </c>
+      <c r="B222">
+        <v>0.9697711650140316</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A223" t="s">
+        <v>10</v>
+      </c>
+      <c r="B223">
+        <v>0.921411876361515</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A224" t="s">
+        <v>10</v>
+      </c>
+      <c r="B224">
+        <v>0.9058232889643244</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A225" t="s">
+        <v>10</v>
+      </c>
+      <c r="B225">
+        <v>0.952449841400138</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A226" t="s">
+        <v>10</v>
+      </c>
+      <c r="B226">
+        <v>0.92064278092431384</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A227" t="s">
+        <v>10</v>
+      </c>
+      <c r="B227">
+        <v>0.89939522729142551</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A228" t="s">
+        <v>10</v>
+      </c>
+      <c r="B228">
+        <v>0.91687705786506268</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A229" t="s">
+        <v>10</v>
+      </c>
+      <c r="B229">
+        <v>0.92593348635421113</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A230" t="s">
+        <v>10</v>
+      </c>
+      <c r="B230">
+        <v>0.94284649725435432</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A231" t="s">
+        <v>10</v>
+      </c>
+      <c r="B231">
+        <v>0.96499812105585892</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A232" t="s">
+        <v>10</v>
+      </c>
+      <c r="B232">
+        <v>0.8818035270297736</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A233" t="s">
+        <v>10</v>
+      </c>
+      <c r="B233">
+        <v>0.9271677149820341</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A234" t="s">
+        <v>10</v>
+      </c>
+      <c r="B234">
+        <v>0.95786011815329675</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A235" t="s">
+        <v>10</v>
+      </c>
+      <c r="B235">
+        <v>0.94032607334928631</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A236" t="s">
+        <v>10</v>
+      </c>
+      <c r="B236">
+        <v>0.91728714202352135</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A237" t="s">
+        <v>10</v>
+      </c>
+      <c r="B237">
+        <v>0.93412014207143967</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A238" t="s">
+        <v>10</v>
+      </c>
+      <c r="B238">
+        <v>0.93727835304354479</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A239" t="s">
+        <v>10</v>
+      </c>
+      <c r="B239">
+        <v>0.95573170953324882</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A240" t="s">
+        <v>10</v>
+      </c>
+      <c r="B240">
+        <v>0.91509921544190231</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A241" t="s">
+        <v>10</v>
+      </c>
+      <c r="B241">
+        <v>0.88184730225393815</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A242" t="s">
+        <v>10</v>
+      </c>
+      <c r="B242">
+        <v>0.98345618415923985</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
40 epochs final model
</commit_message>
<xml_diff>
--- a/LJ Experiments.xlsx
+++ b/LJ Experiments.xlsx
@@ -8,25 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhvan\Documents\GitHub\P4P-Transformer-ASR-for-Dysarthric-Speech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1B234D-51CF-4C50-A14D-48749E609B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7BEDF0-35A4-40DA-838A-B82FBA81C1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="100 epoches" sheetId="1" r:id="rId1"/>
     <sheet name="40 epoches" sheetId="2" r:id="rId2"/>
     <sheet name="40 + 160 epoches" sheetId="3" r:id="rId3"/>
     <sheet name="40 epoches 2.0" sheetId="4" r:id="rId4"/>
-    <sheet name="40 + 200 epoches" sheetId="5" r:id="rId5"/>
-    <sheet name="40 (final base)" sheetId="6" r:id="rId6"/>
-    <sheet name="Learning rate 3" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
+    <sheet name="40 + 200 epoches" sheetId="5" r:id="rId6"/>
+    <sheet name="40 3.0" sheetId="6" r:id="rId7"/>
+    <sheet name="Learning rate 3" sheetId="7" r:id="rId8"/>
+    <sheet name="40 final " sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="20">
   <si>
     <t>&lt;__main__.DisplayOutputs object at 0x7fe956d0d0a0&gt;</t>
   </si>
@@ -77,6 +79,15 @@
   </si>
   <si>
     <t>WER:0.96</t>
+  </si>
+  <si>
+    <t>Model name: LJ_base_40.h5</t>
+  </si>
+  <si>
+    <t>WER:98%</t>
+  </si>
+  <si>
+    <t>Epoch 40</t>
   </si>
 </sst>
 </file>
@@ -3593,7 +3604,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'40 (final base)'!$P$1</c:f>
+              <c:f>'40 3.0'!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3616,7 +3627,7 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>'40 (final base)'!$P$2:$P$41</c:f>
+              <c:f>'40 3.0'!$P$2:$P$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -4759,6 +4770,404 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="824269088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'40 final '!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WER</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40 final '!$P$2:$P$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>5.2051806504872724</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9565765566163811</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4734794299799909</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4371216230229509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6432285093125381</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.760924730453898</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.523583777472727</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3575970390839629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3061349761176879</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.266161055231813</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2016161423288769</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1955858812349149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.226689229916379</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1804349167281889</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.115839579263878</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.0522527262584049</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.087150177696135</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1780733171540629</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0992883816578269</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0584482054022539</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0808402725892909</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0809442155940061</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.096330180071861</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0878686604211869</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.0096888464510929</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.072081390473391</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0796255170101079</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.094251279083718</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1380352851452089</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.076502317283534</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0890796282750539</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.097446472860466</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.0887087189291129</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.091054144781229</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.1352694695338761</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0548884967617791</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.98048093494986244</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99139857291682454</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0219713011656351</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.0230716553217629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F5C2-4067-86D7-7C26401683C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="883328640"/>
+        <c:axId val="883320320"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="883328640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="883320320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="883320320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="883328640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5094,6 +5503,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -8191,6 +8640,522 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9527,6 +10492,141 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>147638</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>72630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A8CEF8A-A276-3E75-B024-651408189DE5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="361951"/>
+          <a:ext cx="4681538" cy="3511154"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>135730</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>135731</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>519113</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A6CBAA9-EF44-CDFA-45A6-463A912D00AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>85740</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C1CC875-EFB4-A647-495A-F587AA96E89B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6877050"/>
+          <a:ext cx="2028840" cy="1266834"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -13308,6 +14408,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9DAB9C-303C-4DB4-B386-D287B13F597B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261AB831-E7E2-489B-93E7-0AC004FB33D1}">
   <dimension ref="A2:E242"/>
   <sheetViews>
@@ -15254,7 +16366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96B391E4-89BA-4AAC-B348-AA6607CB9BDB}">
   <dimension ref="A1:P41"/>
   <sheetViews>
@@ -15607,12 +16719,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD155F7-A315-4D53-8BED-4CB81365EC0F}">
   <dimension ref="A1:P201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -17235,4 +18347,357 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9713221B-5E44-4E95-8EC0-6F341CE7A709}">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>5.2051806504872724</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>3.9565765566163811</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>3.4734794299799909</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3.4371216230229509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>2.6432285093125381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>1.760924730453898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <v>1.523583777472727</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <v>1.3575970390839629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <v>1.3061349761176879</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <v>1.266161055231813</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <v>1.2016161423288769</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O13">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <v>1.1955858812349149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O14">
+        <v>12</v>
+      </c>
+      <c r="P14">
+        <v>1.226689229916379</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O15">
+        <v>13</v>
+      </c>
+      <c r="P15">
+        <v>1.1804349167281889</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="O16">
+        <v>14</v>
+      </c>
+      <c r="P16">
+        <v>1.115839579263878</v>
+      </c>
+    </row>
+    <row r="17" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O17">
+        <v>15</v>
+      </c>
+      <c r="P17">
+        <v>1.0522527262584049</v>
+      </c>
+    </row>
+    <row r="18" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O18">
+        <v>16</v>
+      </c>
+      <c r="P18">
+        <v>1.087150177696135</v>
+      </c>
+    </row>
+    <row r="19" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O19">
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <v>1.1780733171540629</v>
+      </c>
+    </row>
+    <row r="20" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O20">
+        <v>18</v>
+      </c>
+      <c r="P20">
+        <v>1.0992883816578269</v>
+      </c>
+    </row>
+    <row r="21" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O21">
+        <v>19</v>
+      </c>
+      <c r="P21">
+        <v>1.0584482054022539</v>
+      </c>
+    </row>
+    <row r="22" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="P22">
+        <v>1.0808402725892909</v>
+      </c>
+    </row>
+    <row r="23" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O23">
+        <v>21</v>
+      </c>
+      <c r="P23">
+        <v>1.0809442155940061</v>
+      </c>
+    </row>
+    <row r="24" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O24">
+        <v>22</v>
+      </c>
+      <c r="P24">
+        <v>1.096330180071861</v>
+      </c>
+    </row>
+    <row r="25" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O25">
+        <v>23</v>
+      </c>
+      <c r="P25">
+        <v>1.0878686604211869</v>
+      </c>
+    </row>
+    <row r="26" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O26">
+        <v>24</v>
+      </c>
+      <c r="P26">
+        <v>1.0096888464510929</v>
+      </c>
+    </row>
+    <row r="27" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O27">
+        <v>25</v>
+      </c>
+      <c r="P27">
+        <v>1.072081390473391</v>
+      </c>
+    </row>
+    <row r="28" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O28">
+        <v>26</v>
+      </c>
+      <c r="P28">
+        <v>1.0796255170101079</v>
+      </c>
+    </row>
+    <row r="29" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O29">
+        <v>27</v>
+      </c>
+      <c r="P29">
+        <v>1.094251279083718</v>
+      </c>
+    </row>
+    <row r="30" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O30">
+        <v>28</v>
+      </c>
+      <c r="P30">
+        <v>1.1380352851452089</v>
+      </c>
+    </row>
+    <row r="31" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O31">
+        <v>29</v>
+      </c>
+      <c r="P31">
+        <v>1.076502317283534</v>
+      </c>
+    </row>
+    <row r="32" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O32">
+        <v>30</v>
+      </c>
+      <c r="P32">
+        <v>1.0890796282750539</v>
+      </c>
+    </row>
+    <row r="33" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O33">
+        <v>31</v>
+      </c>
+      <c r="P33">
+        <v>1.097446472860466</v>
+      </c>
+    </row>
+    <row r="34" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O34">
+        <v>32</v>
+      </c>
+      <c r="P34">
+        <v>1.0887087189291129</v>
+      </c>
+    </row>
+    <row r="35" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O35">
+        <v>33</v>
+      </c>
+      <c r="P35">
+        <v>1.091054144781229</v>
+      </c>
+    </row>
+    <row r="36" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O36">
+        <v>34</v>
+      </c>
+      <c r="P36">
+        <v>1.1352694695338761</v>
+      </c>
+    </row>
+    <row r="37" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O37">
+        <v>35</v>
+      </c>
+      <c r="P37">
+        <v>1.0548884967617791</v>
+      </c>
+    </row>
+    <row r="38" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O38">
+        <v>36</v>
+      </c>
+      <c r="P38">
+        <v>0.98048093494986244</v>
+      </c>
+    </row>
+    <row r="39" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O39">
+        <v>37</v>
+      </c>
+      <c r="P39">
+        <v>0.99139857291682454</v>
+      </c>
+    </row>
+    <row r="40" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O40">
+        <v>38</v>
+      </c>
+      <c r="P40">
+        <v>1.0219713011656351</v>
+      </c>
+    </row>
+    <row r="41" spans="15:16" x14ac:dyDescent="0.45">
+      <c r="O41">
+        <v>39</v>
+      </c>
+      <c r="P41">
+        <v>1.0230716553217629</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>